<commit_message>
MAde changes to the files for consistency.
MAde changes to the files for consistency.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Account</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>001q000000hmfgoAAA</t>
+  </si>
+  <si>
+    <t>a1Zq0000000EJNA</t>
+  </si>
+  <si>
+    <t>001q000000hmj2V</t>
   </si>
 </sst>
 </file>
@@ -472,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,8 +581,16 @@
       <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have made changes to the test-cases of Repeat Visit
Have made changes to the test-cases of Repeat visit as they were getting failed to value fetch issue.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Account</t>
   </si>
@@ -114,13 +114,40 @@
   </si>
   <si>
     <t>001q000000hmj2V</t>
+  </si>
+  <si>
+    <t>WDStartDate</t>
+  </si>
+  <si>
+    <t>WDEndDate</t>
+  </si>
+  <si>
+    <t>LineType</t>
+  </si>
+  <si>
+    <t>RecordType</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>DeadTime</t>
+  </si>
+  <si>
+    <t>ScheduledDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +176,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,7 +199,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -179,8 +211,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,18 +227,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,10 +541,16 @@
     <col min="9" max="9" width="41.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="41.83203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="34" style="3" customWidth="1"/>
+    <col min="13" max="13" width="43.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="30" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="28.5" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,8 +584,26 @@
       <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -567,8 +637,26 @@
       <c r="K2" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="L2" s="5">
+        <v>42999.416666666664</v>
+      </c>
+      <c r="M2" s="5">
+        <v>42999.583333333336</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>42999</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -588,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added MTTR test-cases and made changes to old ones.
Added MTTR test-cases and made changes to old ones.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Account</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>ScheduledDate</t>
+  </si>
+  <si>
+    <t>2017-09-21 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-09-21 13:00:00</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -215,8 +221,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -230,11 +238,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -242,6 +253,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -249,6 +261,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,8 +554,8 @@
     <col min="9" max="9" width="41.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="41.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="34" style="3" customWidth="1"/>
-    <col min="13" max="13" width="43.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="34" style="5" customWidth="1"/>
+    <col min="13" max="13" width="43.6640625" style="5" customWidth="1"/>
     <col min="14" max="14" width="30" style="1" customWidth="1"/>
     <col min="15" max="15" width="29.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="26.5" style="1" customWidth="1"/>
@@ -584,10 +597,10 @@
       <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -637,11 +650,11 @@
       <c r="K2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="5">
-        <v>42999.416666666664</v>
-      </c>
-      <c r="M2" s="5">
-        <v>42999.583333333336</v>
+      <c r="L2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Added the test-cases for MTTR.
Added the test-cases for MTTR.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Account</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>2017-09-21 13:00:00</t>
+  </si>
+  <si>
+    <t>Parts</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,6 +691,9 @@
       <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
Adding some changes to the test-cases
Adding some changes to the test-cases.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -59,9 +59,6 @@
     <t>01tq0000001jh3s</t>
   </si>
   <si>
-    <t>a0Nq0000003PBZS</t>
-  </si>
-  <si>
     <t>System.Today()</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>01tq0000001jhI0</t>
   </si>
   <si>
-    <t>a0Nq0000003PBEa</t>
-  </si>
-  <si>
     <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed', SVMXC__Priority__c = 'High' );insert SR_1 ;</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>PreferredEndDate</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PF2Z</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PF2e</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,16 +602,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -620,36 +620,36 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -658,40 +658,40 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -700,38 +700,38 @@
         <v>42999</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to test-cases - Tech Utilization
Made changes to test-cases - Tech Utilization
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Account</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>a0Nq0000003PF2e</t>
+  </si>
+  <si>
+    <t>GuaranteedUptime</t>
+  </si>
+  <si>
+    <t>TotalUptime</t>
   </si>
 </sst>
 </file>
@@ -220,7 +226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -242,8 +248,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,8 +271,11 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -275,6 +286,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -285,6 +297,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,10 +598,12 @@
     <col min="17" max="17" width="28.5" style="1" customWidth="1"/>
     <col min="18" max="18" width="42.33203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="28.5" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="25.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="28.1640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,8 +661,14 @@
       <c r="S1" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -705,8 +726,14 @@
       <c r="S2" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="T2" s="7">
+        <v>44640</v>
+      </c>
+      <c r="U2" s="1">
+        <v>44280</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -729,7 +756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Adding Test-cases to Tech Util
Adding Test-cases to Tech Util
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Account</t>
   </si>
@@ -165,6 +165,18 @@
   </si>
   <si>
     <t>TotalUptime</t>
+  </si>
+  <si>
+    <t>SystemStartDate</t>
+  </si>
+  <si>
+    <t>SystemEndDate</t>
+  </si>
+  <si>
+    <t>System.Today() 10:00:00</t>
+  </si>
+  <si>
+    <t>System.Today 16:00:00</t>
   </si>
 </sst>
 </file>
@@ -226,7 +238,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -250,8 +262,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -271,11 +287,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -287,6 +300,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -298,6 +313,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,10 +617,12 @@
     <col min="19" max="19" width="28.5" style="1" customWidth="1"/>
     <col min="20" max="20" width="25.1640625" style="1" customWidth="1"/>
     <col min="21" max="21" width="28.1640625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="1"/>
+    <col min="22" max="22" width="41.5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="29.5" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,8 +686,14 @@
       <c r="U1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -726,14 +751,20 @@
       <c r="S2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="7">
+      <c r="T2" s="1">
         <v>44640</v>
       </c>
       <c r="U2" s="1">
         <v>44280</v>
       </c>
+      <c r="V2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -756,7 +787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'upstream/master'"
This reverts commit 372b71b404b2e0c2755457d8c9fb6d2670ee4baa.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Account</t>
   </si>
@@ -59,9 +59,6 @@
     <t>01tq0000001jh3s</t>
   </si>
   <si>
-    <t>a0Nq0000003PBZS</t>
-  </si>
-  <si>
     <t>System.Today()</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>01tq0000001jhI0</t>
   </si>
   <si>
-    <t>a0Nq0000003PBEa</t>
-  </si>
-  <si>
     <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed', SVMXC__Priority__c = 'High' );insert SR_1 ;</t>
   </si>
   <si>
@@ -147,6 +141,24 @@
   </si>
   <si>
     <t>Parts</t>
+  </si>
+  <si>
+    <t>2017-09-10 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-09-10 16:00:00</t>
+  </si>
+  <si>
+    <t>PreferredStartDate</t>
+  </si>
+  <si>
+    <t>PreferredEndDate</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PF2Z</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PF2e</t>
   </si>
 </sst>
 </file>
@@ -208,8 +220,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -248,7 +264,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -257,6 +273,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -265,6 +283,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,10 +583,12 @@
     <col min="15" max="15" width="29.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="26.5" style="1" customWidth="1"/>
     <col min="17" max="17" width="28.5" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="42.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="28.5" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,16 +602,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -598,30 +620,36 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -630,40 +658,40 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -671,33 +699,39 @@
       <c r="Q2" s="4">
         <v>42999</v>
       </c>
+      <c r="R2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made to the sheet
Changes made to the sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -59,9 +59,6 @@
     <t>01tq0000001jh3s</t>
   </si>
   <si>
-    <t>a0Nq0000003PBZS</t>
-  </si>
-  <si>
     <t>System.Today()</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>01tq0000001jhI0</t>
   </si>
   <si>
-    <t>a0Nq0000003PBEa</t>
-  </si>
-  <si>
     <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed', SVMXC__Priority__c = 'High' );insert SR_1 ;</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>PreferredEndDate</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PKUh</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PKUc</t>
   </si>
 </sst>
 </file>
@@ -220,8 +220,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -264,7 +266,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -275,6 +277,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -285,6 +288,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,16 +606,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -620,36 +624,36 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -658,40 +662,40 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -700,38 +704,38 @@
         <v>42999</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to the data sheet
Made changes to the data sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -56,9 +56,6 @@
     <t>a1Jq0000001fK4a</t>
   </si>
   <si>
-    <t>01tq0000001jh3s</t>
-  </si>
-  <si>
     <t>System.Today()</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>a0Nq0000003PKUc</t>
+  </si>
+  <si>
+    <t>01tq0000001jgnm</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,16 +606,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -624,78 +624,78 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -704,38 +704,38 @@
         <v>42999</v>
       </c>
       <c r="R2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to test cases of ART and MTTC and Contract Uptime
Made changes to test cases of ART and MTTC and Contract Uptime
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Account</t>
   </si>
@@ -155,10 +155,13 @@
     <t>PreferredEndDate</t>
   </si>
   <si>
-    <t>a0Nq0000003PF2Z</t>
-  </si>
-  <si>
-    <t>a0Nq0000003PF2e</t>
+    <t>a0Nq0000003PKUc</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PKUh</t>
+  </si>
+  <si>
+    <t>GuranteedUptime</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,6 +205,11 @@
       <color rgb="FF454545"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +228,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -242,8 +250,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,8 +273,9 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -275,6 +286,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -285,6 +297,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,10 +598,11 @@
     <col min="17" max="17" width="28.5" style="1" customWidth="1"/>
     <col min="18" max="18" width="42.33203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="28.5" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="41" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,8 +660,11 @@
       <c r="S1" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="T1" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -705,8 +722,11 @@
       <c r="S2" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="T2" s="1">
+        <v>44640</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -729,7 +749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Made Changes to Datasheet
Made Changes to Datasheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -56,9 +56,6 @@
     <t>a1Jq0000001fK4a</t>
   </si>
   <si>
-    <t>01tq0000001jh3s</t>
-  </si>
-  <si>
     <t>System.Today()</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>GuranteedUptime</t>
+  </si>
+  <si>
+    <t>01tq000000081s5</t>
   </si>
 </sst>
 </file>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,16 +616,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -634,81 +634,81 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="T1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -717,10 +717,10 @@
         <v>42999</v>
       </c>
       <c r="R2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="T2" s="1">
         <v>44640</v>
@@ -728,30 +728,30 @@
     </row>
     <row r="3" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to Contract Uptime
Made changes to Contract Uptime
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -131,21 +131,9 @@
     <t>ScheduledDate</t>
   </si>
   <si>
-    <t>2017-09-21 10:00:00</t>
-  </si>
-  <si>
-    <t>2017-09-21 13:00:00</t>
-  </si>
-  <si>
     <t>Parts</t>
   </si>
   <si>
-    <t>2017-09-10 10:00:00</t>
-  </si>
-  <si>
-    <t>2017-09-10 16:00:00</t>
-  </si>
-  <si>
     <t>PreferredStartDate</t>
   </si>
   <si>
@@ -162,6 +150,18 @@
   </si>
   <si>
     <t>01tq000000081s5</t>
+  </si>
+  <si>
+    <t>2017-10-10 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-10-10 16:00:00</t>
+  </si>
+  <si>
+    <t>2017-10-21 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-10-21 13:00:00</t>
   </si>
 </sst>
 </file>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,13 +655,13 @@
         <v>33</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="112" customHeight="1" x14ac:dyDescent="0.2">
@@ -672,10 +672,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -699,10 +699,10 @@
         <v>18</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>30</v>
@@ -714,13 +714,13 @@
         <v>30</v>
       </c>
       <c r="Q2" s="4">
-        <v>42999</v>
+        <v>43029</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="T2" s="1">
         <v>44640</v>
@@ -737,7 +737,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>24</v>
@@ -746,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Made changes to the username and pwd
Made changes to the username and pwd
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Account</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>2017-10-21 13:00:00</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>meghana.rao@servicemax.com</t>
+  </si>
+  <si>
+    <t>cloud_101</t>
   </si>
 </sst>
 </file>
@@ -573,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,10 +611,12 @@
     <col min="18" max="18" width="42.33203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="28.5" style="1" customWidth="1"/>
     <col min="20" max="20" width="41" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="52.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,8 +677,14 @@
       <c r="T1" s="7" t="s">
         <v>39</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -725,8 +745,14 @@
       <c r="T2" s="1">
         <v>44640</v>
       </c>
+      <c r="U2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -749,7 +775,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Changed to ContractUptime test-case
Changed to ContractUptime test-case
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanarao/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Account</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>cloud_101</t>
+  </si>
+  <si>
+    <t>DownTime</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,10 +636,11 @@
     <col min="20" max="20" width="41" style="1" customWidth="1"/>
     <col min="21" max="21" width="15.83203125" style="1" customWidth="1"/>
     <col min="22" max="22" width="19.6640625" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="23" max="23" width="28.33203125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,8 +707,11 @@
       <c r="V1" s="8" t="s">
         <v>46</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -771,8 +778,11 @@
       <c r="V2" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="W2" s="1">
+        <v>360</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -795,7 +805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Made changes to test-cases
Made changes to test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Account</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>DownTime</t>
+  </si>
+  <si>
+    <t>UptimeValue</t>
   </si>
 </sst>
 </file>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,10 +640,11 @@
     <col min="21" max="21" width="15.83203125" style="1" customWidth="1"/>
     <col min="22" max="22" width="19.6640625" style="1" customWidth="1"/>
     <col min="23" max="23" width="28.33203125" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="1"/>
+    <col min="24" max="24" width="25.33203125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,8 +714,11 @@
       <c r="W1" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -781,8 +788,11 @@
       <c r="W2" s="1">
         <v>360</v>
       </c>
+      <c r="X2" s="7">
+        <v>98.33</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -805,7 +815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Changes made to test-case
Changes made to test-case
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanarao/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -152,18 +152,6 @@
     <t>01tq000000081s5</t>
   </si>
   <si>
-    <t>2017-10-21 10:00:00</t>
-  </si>
-  <si>
-    <t>2017-10-21 13:00:00</t>
-  </si>
-  <si>
-    <t>2017-11-10 16:00:00</t>
-  </si>
-  <si>
-    <t>2017-11-10 10:00:00</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -180,6 +168,18 @@
   </si>
   <si>
     <t>UptimeValue</t>
+  </si>
+  <si>
+    <t>2017-12-21 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-12-21 13:00:00</t>
+  </si>
+  <si>
+    <t>2017-12-10 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-12-10 16:00:00</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,16 +725,16 @@
         <v>39</v>
       </c>
       <c r="U1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="Y1" s="10"/>
     </row>
@@ -773,10 +773,10 @@
         <v>18</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>30</v>
@@ -788,22 +788,22 @@
         <v>30</v>
       </c>
       <c r="Q2" s="4">
-        <v>43060</v>
+        <v>43121</v>
       </c>
       <c r="R2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="1">
+        <v>44640</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" s="1">
-        <v>43200</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="W2" s="1">
         <v>360</v>

</xml_diff>

<commit_message>
Making changes to the test-cases
Making changes to the test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Account</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>2017-12-10 16:00:00</t>
+  </si>
+  <si>
+    <t>user_meghana</t>
+  </si>
+  <si>
+    <t>005q0000003GGfP</t>
   </si>
 </sst>
 </file>
@@ -263,8 +269,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -323,7 +333,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -339,6 +349,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -354,6 +366,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -631,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +750,9 @@
       <c r="X1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="10"/>
+      <c r="Y1" s="10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="2" spans="1:25" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -811,7 +827,9 @@
       <c r="X2" s="7">
         <v>98.33</v>
       </c>
-      <c r="Y2" s="10"/>
+      <c r="Y2" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:25" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
Adding changes to Attach Rate test-cases
Adding changes to Attach Rate test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Made changes to the test-cases 1
Made changes to the test-cases 1
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Account</t>
   </si>
@@ -44,24 +44,15 @@
     <t>InsertCase</t>
   </si>
   <si>
-    <t>Closed</t>
-  </si>
-  <si>
     <t>Case case_1 = new Case (Status = 'Closed' );insert case_1 ;</t>
   </si>
   <si>
     <t>Site</t>
   </si>
   <si>
-    <t>a1Jq0000001fK4a</t>
-  </si>
-  <si>
     <t>System.Today()</t>
   </si>
   <si>
-    <t>a1Zq0000001jyS9</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -77,33 +68,15 @@
     <t>SubStatus</t>
   </si>
   <si>
-    <t>OrderStatus</t>
-  </si>
-  <si>
     <t>InsertServiceRequest</t>
   </si>
   <si>
     <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Open' );insert SR_1 ;</t>
   </si>
   <si>
-    <t>a1Jq0000001faAI</t>
-  </si>
-  <si>
-    <t>01tq0000001jhI0</t>
-  </si>
-  <si>
     <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed', SVMXC__Priority__c = 'High' );insert SR_1 ;</t>
   </si>
   <si>
-    <t>001q000000hmXhAAAU</t>
-  </si>
-  <si>
-    <t>001q000000hmfgoAAA</t>
-  </si>
-  <si>
-    <t>001q000000hmj2V</t>
-  </si>
-  <si>
     <t>WDStartDate</t>
   </si>
   <si>
@@ -137,18 +110,9 @@
     <t>PreferredEndDate</t>
   </si>
   <si>
-    <t>a0Nq0000003PKUc</t>
-  </si>
-  <si>
-    <t>a0Nq0000003PKUh</t>
-  </si>
-  <si>
     <t>GuranteedUptime</t>
   </si>
   <si>
-    <t>01tq000000081s5</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -185,7 +149,10 @@
     <t>005q0000003GGfP</t>
   </si>
   <si>
-    <t>a2N1g000000EWS4</t>
+    <t>workinghours</t>
+  </si>
+  <si>
+    <t>01mo0000000K7kC</t>
   </si>
 </sst>
 </file>
@@ -269,8 +236,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,7 +306,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -354,6 +325,8 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -372,6 +345,8 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1:Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,10 +634,9 @@
     <col min="2" max="2" width="42.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
     <col min="6" max="8" width="37.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="41.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="41.83203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="34" style="5" customWidth="1"/>
     <col min="13" max="13" width="43.6640625" style="5" customWidth="1"/>
@@ -678,10 +652,11 @@
     <col min="23" max="23" width="28.33203125" style="1" customWidth="1"/>
     <col min="24" max="24" width="25.33203125" style="1" customWidth="1"/>
     <col min="25" max="25" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="1"/>
+    <col min="26" max="26" width="41.33203125" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,114 +670,97 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="2"/>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="112" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -811,19 +769,19 @@
         <v>43121</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="T2" s="1">
         <v>44640</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="W2" s="1">
         <v>360</v>
@@ -832,34 +790,17 @@
         <v>98.33</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>51</v>
+        <v>39</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>52</v>
-      </c>
+    <row r="3" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="K3" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made changes to the test-case
Made changes to the test-case
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Account</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>01mo0000000K7kC</t>
+  </si>
+  <si>
+    <t>OrderStatus</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -622,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,24 +641,24 @@
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="37.6640625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="37.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="41.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="41.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="34" style="5" customWidth="1"/>
-    <col min="13" max="13" width="43.6640625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="30" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="28.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="42.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="28.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="41" style="1" customWidth="1"/>
-    <col min="21" max="21" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="28.33203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="25.33203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="41.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="34" style="5" customWidth="1"/>
+    <col min="12" max="12" width="43.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="30" style="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="26.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="42.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="28.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41" style="1" customWidth="1"/>
+    <col min="20" max="20" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="28.33203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="25.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="41.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="54.5" style="1" customWidth="1"/>
     <col min="27" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -673,15 +679,18 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -736,15 +745,18 @@
     <row r="2" spans="1:26" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="2"/>
       <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -796,13 +808,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="96" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="M3" s="5"/>
       <c r="N3" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="F4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made changes to an_Datasheet1
Made changes to an_Datasheet1
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanarao/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Account</t>
   </si>
@@ -149,40 +149,49 @@
     <t>Closed</t>
   </si>
   <si>
-    <t>meghana.rao@upgrade_ge.com</t>
-  </si>
-  <si>
-    <t>salesforce100</t>
-  </si>
-  <si>
-    <t>0050x000000ZMuv</t>
-  </si>
-  <si>
-    <t>01mi0000000ISUq</t>
-  </si>
-  <si>
-    <t>a250x000000SDdqAAG</t>
-  </si>
-  <si>
-    <t>a250x000000SDdvAAG</t>
-  </si>
-  <si>
-    <t>0010x000007lNeNAAU</t>
-  </si>
-  <si>
-    <t>0010x000007lNeXAAU</t>
-  </si>
-  <si>
-    <t>01t0x000000KU1qAAG</t>
-  </si>
-  <si>
-    <t>01t0x000000KU1vAAG</t>
-  </si>
-  <si>
-    <t>a0T0x0000000iUxEAI</t>
-  </si>
-  <si>
-    <t>a2N0x000000BzUAEA0</t>
+    <t>meghana.rao@servicemax.com</t>
+  </si>
+  <si>
+    <t>cloud_101</t>
+  </si>
+  <si>
+    <t>005q0000003GGfP</t>
+  </si>
+  <si>
+    <t>01mo0000000K7kC</t>
+  </si>
+  <si>
+    <t>001q000000hmXhAAAU</t>
+  </si>
+  <si>
+    <t>a1Jq0000001fK4a</t>
+  </si>
+  <si>
+    <t>01tq000000081s5</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PKUc</t>
+  </si>
+  <si>
+    <t>001q000000hmfgoAAA</t>
+  </si>
+  <si>
+    <t>a1Jq0000001faAI</t>
+  </si>
+  <si>
+    <t>01tq0000001jhI0</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PKUh</t>
+  </si>
+  <si>
+    <t>001q000000hmj2V</t>
+  </si>
+  <si>
+    <t>a1Zq0000001jyS9</t>
+  </si>
+  <si>
+    <t>a2N1g000000EWS4</t>
   </si>
 </sst>
 </file>
@@ -266,7 +275,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -310,8 +319,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -337,8 +347,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -381,6 +392,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -659,7 +671,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +694,7 @@
     <col min="18" max="18" width="28.5" style="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="41" style="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="29.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="90.6640625" style="1" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="25.33203125" style="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="30.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
@@ -772,20 +784,20 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="112" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>39</v>
@@ -832,7 +844,7 @@
       <c r="T2" s="1">
         <v>44640</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="11" t="s">
         <v>40</v>
       </c>
       <c r="V2" s="10" t="s">
@@ -852,20 +864,20 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="96" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F3" s="1"/>
       <c r="J3" s="1"/>
@@ -879,13 +891,18 @@
       <c r="Z3"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B4"/>
+      <c r="A4" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="U2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding changes for MTTR Suite
Adding changes for MTTR Suite
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Account</t>
   </si>
@@ -159,39 +159,6 @@
   </si>
   <si>
     <t>01mo0000000K7kC</t>
-  </si>
-  <si>
-    <t>001q000000hmXhAAAU</t>
-  </si>
-  <si>
-    <t>a1Jq0000001fK4a</t>
-  </si>
-  <si>
-    <t>01tq000000081s5</t>
-  </si>
-  <si>
-    <t>a0Nq0000003PKUc</t>
-  </si>
-  <si>
-    <t>001q000000hmfgoAAA</t>
-  </si>
-  <si>
-    <t>a1Jq0000001faAI</t>
-  </si>
-  <si>
-    <t>01tq0000001jhI0</t>
-  </si>
-  <si>
-    <t>a0Nq0000003PKUh</t>
-  </si>
-  <si>
-    <t>001q000000hmj2V</t>
-  </si>
-  <si>
-    <t>a1Zq0000001jyS9</t>
-  </si>
-  <si>
-    <t>a2N1g000000EWS4</t>
   </si>
 </sst>
 </file>
@@ -671,7 +638,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,21 +751,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="112" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="F2" s="1" t="s">
         <v>39</v>
       </c>
@@ -864,21 +817,6 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="96" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
@@ -891,9 +829,6 @@
       <c r="Z3"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added changes to the test-cases
Added changes to the test-cases
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Account</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>01mo0000000K7kC</t>
+  </si>
+  <si>
+    <t>ServiceTeam</t>
+  </si>
+  <si>
+    <t>a1Nq0000000RlgV</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -287,6 +293,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -316,7 +323,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -338,6 +345,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -635,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E5"/>
+      <selection activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,29 +656,30 @@
     <col min="3" max="3" width="43" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="20.83203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="37.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="34" style="5" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="43.6640625" style="5" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="30" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="29.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="26.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="28.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="42.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="28.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="41" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="29.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="90.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="25.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="30.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="41.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="54.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="16384" width="10.83203125" style="1" collapsed="1"/>
+    <col min="6" max="6" width="20.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="37.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="41.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="34" style="5" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="43.6640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="30" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="29.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="28.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="42.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="41" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="29.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="90.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="30.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="41.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="54.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,156 +696,165 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+      <c r="C2"/>
       <c r="D2" s="2"/>
       <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>30</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>43121</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>44640</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>360</v>
       </c>
-      <c r="X2" s="7">
+      <c r="Y2" s="7">
         <v>98.33</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="96" x14ac:dyDescent="0.2">
-      <c r="F3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
+    <row r="3" spans="1:27" ht="96" x14ac:dyDescent="0.2">
+      <c r="A3"/>
+      <c r="G3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z3"/>
+      <c r="AA3"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Modified references and updated the cache reset to true
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/an_Datasheet1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanarao/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/auto/sahi_pro/userdata/scripts/Sahi_Project/svmx/test_lab/test_cases/analytics/an_excleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -152,9 +152,6 @@
     <t>meghana.rao@servicemax.com</t>
   </si>
   <si>
-    <t>cloud_101</t>
-  </si>
-  <si>
     <t>005q0000003GGfP</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>a1Zq0000001ktdZEAQ</t>
+  </si>
+  <si>
+    <t>cloud_102</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,11 +246,6 @@
       <color rgb="FF3933FF"/>
       <name val="Monaco"/>
     </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF263238"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,7 +264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -313,10 +308,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,10 +335,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -366,7 +358,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -388,7 +380,6 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -666,38 +657,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="36.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="42.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="43.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="20.83203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="20.83203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.6640625" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="1" width="37.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="41.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="5" width="34.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="5" width="43.6640625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="1" width="30.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="1" width="29.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="1" width="26.5" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="1" width="28.5" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="1" width="42.33203125" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="28.5" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="1" width="41.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="29.6640625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="1" width="90.6640625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="1" width="25.33203125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="30.83203125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="1" width="41.33203125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="1" width="54.5" collapsed="true"/>
-    <col min="28" max="16384" style="1" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="20.83203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="37.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="41.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="34" style="5" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="43.6640625" style="5" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="30" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="29.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="28.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="42.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="41" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="29.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="90.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="28.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="30.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="41.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="54.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
@@ -717,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>38</v>
@@ -785,22 +775,22 @@
     </row>
     <row r="2" spans="1:27" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>39</v>
@@ -847,11 +837,11 @@
       <c r="U2" s="1">
         <v>44640</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="10" t="s">
-        <v>41</v>
+      <c r="W2" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="X2" s="1">
         <v>360</v>
@@ -860,27 +850,27 @@
         <v>98.33</v>
       </c>
       <c r="Z2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" t="s">
         <v>42</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
       </c>
       <c r="G3" s="1"/>
       <c r="K3" s="1"/>
@@ -900,9 +890,6 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>